<commit_message>
update metadata template and sample accession regex
</commit_message>
<xml_diff>
--- a/eva_sub_cli/etc/EVA_Submission_template.xlsx
+++ b/eva_sub_cli/etc/EVA_Submission_template.xlsx
@@ -35,7 +35,7 @@
     <t xml:space="preserve">PLEASE READ FIRST</t>
   </si>
   <si>
-    <t xml:space="preserve">V2.0.0 Mar 2025</t>
+    <t xml:space="preserve">V2.0.1 May 2025</t>
   </si>
   <si>
     <t xml:space="preserve">This Spreadsheet is meant to be used with the EVA submissions command line tools eva-sub-cli.</t>
@@ -395,13 +395,13 @@
     <t xml:space="preserve">Imputation</t>
   </si>
   <si>
-    <t xml:space="preserve">Enter '1' if this was an imputation analysis. NOTE: the single quotes should be included.</t>
+    <t xml:space="preserve">Enter '1' if this was an imputation analysis, otherwise leave blank</t>
   </si>
   <si>
     <t xml:space="preserve">Phasing</t>
   </si>
   <si>
-    <t xml:space="preserve">Enter '1' if this was a phased analysis. NOTE: the single quotes should be included.</t>
+    <t xml:space="preserve">Enter '1' if this was a phased analysis, otherwise leave blank</t>
   </si>
   <si>
     <t xml:space="preserve">Centre</t>
@@ -494,7 +494,7 @@
     <t xml:space="preserve">Sample Accession</t>
   </si>
   <si>
-    <t xml:space="preserve">BioSample Accession of For Pre Existing sample. Only use for preregistered samples</t>
+    <t xml:space="preserve">BioSample accession of pre-existing sample. Only use for preregistered samples</t>
   </si>
   <si>
     <t xml:space="preserve">Section 3: "Novel sample(s)"</t>
@@ -16841,7 +16841,7 @@
   <dimension ref="A1:AT1003"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>